<commit_message>
added full scip results to archive
</commit_message>
<xml_diff>
--- a/data/archive/scip/results.xlsx
+++ b/data/archive/scip/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3344" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="1218">
   <si>
     <t xml:space="preserve">Run Time</t>
   </si>
@@ -3185,6 +3185,495 @@
   </si>
   <si>
     <t xml:space="preserve">d1=0.280097, d2=0.772538, d3=0.224634, d4=0.252969, d5=0.093870, d6=0.181375, d7=0.495015, d8=0.253002, d9=0.554320, d10=0.772538, d11=0.702294, d12=0.221580, d13=0.093870, d14=0.869434, d15=0.306586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 01:37:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters3_points16_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.216891, cluster_1_dim_2=-0.441918, cluster_1_dim_3=-0.187265, cluster_1_dim_4=0.588570, cluster_1_dim_5=0.162106, cluster_2_dim_1=0.504081, cluster_2_dim_2=-0.126319, cluster_2_dim_3=-0.406057, cluster_2_dim_4=-0.346150, cluster_2_dim_5=-0.439230, cluster_3_dim_1=0.504081, cluster_3_dim_2=0.562547, cluster_3_dim_3=0.784503, cluster_3_dim_4=0.388360, cluster_3_dim_5=0.553297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.684915, d2=1.057096, d3=0.734382, d4=0.418325, d5=0.648090, d6=0.316963, d7=0.878379, d8=0.724991, d9=1.288261, d10=1.464422, d11=1.778981, d12=0.663374, d13=0.465558, d14=0.993796, d15=2.477589, d16=0.866057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 02:07:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.047459, cluster_1_dim_2=-0.724349, cluster_1_dim_3=0.009646, cluster_1_dim_4=0.092517, cluster_1_dim_5=-0.396924, cluster_2_dim_1=0.380757, cluster_2_dim_2=0.562547, cluster_2_dim_3=0.784503, cluster_2_dim_4=0.388360, cluster_2_dim_5=0.553297, cluster_3_dim_1=0.514703, cluster_3_dim_2=0.160850, cluster_3_dim_3=-0.606093, cluster_3_dim_4=-0.054493, cluster_3_dim_5=-0.045967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.806661, d2=1.161706, d3=1.008072, d4=0.549733, d5=0.767574, d6=0.281542, d7=0.757884, d8=0.692007, d9=2.013452, d10=1.178785, d11=1.237958, d12=0.983366, d13=0.335869, d14=0.425286, d15=2.410500, d16=1.608688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 02:37:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.216891, cluster_1_dim_2=-0.441918, cluster_1_dim_3=-0.187265, cluster_1_dim_4=0.588570, cluster_1_dim_5=0.162106, cluster_2_dim_1=0.504081, cluster_2_dim_2=-0.269018, cluster_2_dim_3=-0.452425, cluster_2_dim_4=-0.416318, cluster_2_dim_5=-0.423000, cluster_3_dim_1=0.504081, cluster_3_dim_2=0.640053, cluster_3_dim_3=0.568007, cluster_3_dim_4=0.327527, cluster_3_dim_5=0.276762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.679715, d2=1.057096, d3=0.694416, d4=0.375536, d5=0.380279, d6=0.763702, d7=0.708934, d8=0.585058, d9=1.288261, d10=1.304577, d11=1.778981, d12=0.636707, d13=0.685780, d14=1.223897, d15=2.477589, d16=0.866057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 03:07:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.216891, cluster_1_dim_2=-0.441918, cluster_1_dim_3=-0.187265, cluster_1_dim_4=0.588570, cluster_1_dim_5=0.162106, cluster_2_dim_1=0.380757, cluster_2_dim_2=0.562547, cluster_2_dim_3=0.784503, cluster_2_dim_4=0.388360, cluster_2_dim_5=0.553297, cluster_3_dim_1=0.550328, cluster_3_dim_2=-0.126319, cluster_3_dim_3=-0.406057, cluster_3_dim_4=-0.346150, cluster_3_dim_5=-0.439230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.793442, d2=1.057096, d3=0.725289, d4=0.378457, d5=0.767574, d6=0.281542, d7=0.864786, d8=0.737816, d9=1.288261, d10=1.436287, d11=1.778981, d12=0.642476, d13=0.335869, d14=0.966920, d15=2.477589, d16=0.866057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 03:37:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters4_points15_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.591837, cluster_1_dim_2=0.711375, cluster_1_dim_3=0.041505, cluster_1_dim_4=0.011950, cluster_1_dim_5=0.560220, cluster_2_dim_1=-0.553288, cluster_2_dim_2=-0.576948, cluster_2_dim_3=-0.712242, cluster_2_dim_4=0.051587, cluster_2_dim_5=0.223049, cluster_3_dim_1=0.452604, cluster_3_dim_2=0.397458, cluster_3_dim_3=0.482816, cluster_3_dim_4=0.177160, cluster_3_dim_5=-0.361507, cluster_4_dim_1=0.770082, cluster_4_dim_2=-0.360538, cluster_4_dim_3=-0.201517, cluster_4_dim_4=0.088720, cluster_4_dim_5=0.689148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.522683, d2=0.753412, d3=0.756730, d4=0.971822, d5=0.424433, d6=1.023904, d7=0.462893, d8=0.818327, d9=0.378499, d10=0.095335, d11=1.798758, d12=0.280767, d13=0.608966, d14=0.355449, d15=0.843984</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 04:07:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.722772, cluster_1_dim_2=-0.667387, cluster_1_dim_3=-0.809180, cluster_1_dim_4=0.281151, cluster_1_dim_5=0.138741, cluster_2_dim_1=-0.285637, cluster_2_dim_2=0.760705, cluster_2_dim_3=0.199935, cluster_2_dim_4=-0.059594, cluster_2_dim_5=0.462938, cluster_3_dim_1=0.407514, cluster_3_dim_2=0.269648, cluster_3_dim_3=0.434713, cluster_3_dim_4=0.290007, cluster_3_dim_5=-0.494657, cluster_4_dim_1=0.573201, cluster_4_dim_2=-0.367645, cluster_4_dim_3=-0.264887, cluster_4_dim_4=-0.010532, cluster_4_dim_5=0.629651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.785114, d2=0.891196, d3=0.771566, d4=0.681156, d5=0.899506, d6=0.833730, d7=0.399895, d8=1.222873, d9=0.691743, d10=0.252713, d11=1.616331, d12=0.368147, d13=0.376099, d14=0.376099, d15=1.025115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 04:37:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 05:07:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.553288, cluster_1_dim_2=-0.576948, cluster_1_dim_3=-0.712242, cluster_1_dim_4=0.051587, cluster_1_dim_5=0.223049, cluster_2_dim_1=-0.390036, cluster_2_dim_2=0.754649, cluster_2_dim_3=-0.083515, cluster_2_dim_4=0.233834, cluster_2_dim_5=0.251796, cluster_3_dim_1=0.520818, cluster_3_dim_2=0.267839, cluster_3_dim_3=0.641737, cluster_3_dim_4=-0.031766, cluster_3_dim_5=-0.067885, cluster_4_dim_1=0.841298, cluster_4_dim_2=-0.559510, cluster_4_dim_3=-0.380701, cluster_4_dim_4=0.166674, cluster_4_dim_5=0.653985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.687766, d2=0.498097, d3=0.852509, d4=1.229112, d5=0.424433, d6=0.861893, d7=1.086365, d8=0.540294, d9=0.264995, d10=0.193119, d11=1.823259, d12=0.121740, d13=0.608966, d14=0.355449, d15=0.787192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 05:37:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters5_points14_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.561261, cluster_1_dim_2=0.646714, cluster_1_dim_3=0.598294, cluster_1_dim_4=-0.379994, cluster_1_dim_5=-0.280810, cluster_2_dim_1=-0.270913, cluster_2_dim_2=-0.604444, cluster_2_dim_3=-0.288663, cluster_2_dim_4=-0.207101, cluster_2_dim_5=-0.163442, cluster_3_dim_1=0.332521, cluster_3_dim_2=-0.143714, cluster_3_dim_3=-0.536338, cluster_3_dim_4=0.410118, cluster_3_dim_5=0.753828, cluster_4_dim_1=0.564770, cluster_4_dim_2=0.554241, cluster_4_dim_3=0.505835, cluster_4_dim_4=0.307723, cluster_4_dim_5=0.119407, cluster_5_dim_1=0.619351, cluster_5_dim_2=0.853743, cluster_5_dim_3=-0.529514, cluster_5_dim_4=-0.925581, cluster_5_dim_5=0.664433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.431664, d2=0.504344, d3=0.748873, d4=0.256210, d5=0.256210, d6=0.919398, d7=0.238304, d8=0.286995, d9=0.400669, d10=0.286995, d11=0.705751, d12=0.238304, d13=0.210438, d14=0.456414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 06:07:56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=0.012322, cluster_1_dim_2=0.853743, cluster_1_dim_3=-0.529514, cluster_1_dim_4=-0.925581, cluster_1_dim_5=0.664433, cluster_2_dim_1=0.012322, cluster_2_dim_2=0.661251, cluster_2_dim_3=0.501773, cluster_2_dim_4=0.063536, cluster_2_dim_5=-0.315055, cluster_3_dim_1=0.012322, cluster_3_dim_2=0.399626, cluster_3_dim_3=0.806151, cluster_3_dim_4=-0.619669, cluster_3_dim_5=0.149705, cluster_4_dim_1=0.012322, cluster_4_dim_2=-0.604444, cluster_4_dim_3=-0.288663, cluster_4_dim_4=-0.207101, cluster_4_dim_5=-0.163442, cluster_5_dim_1=0.413470, cluster_5_dim_2=0.136962, cluster_5_dim_3=-0.259108, cluster_5_dim_4=0.484269, cluster_5_dim_5=0.712637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.677530, d2=0.308918, d3=0.879179, d4=0.400793, d5=0.272071, d6=0.913057, d7=0.274937, d8=0.829973, d9=0.822925, d10=0.480986, d11=1.235152, d12=0.540436, d13=0.326061, d14=1.031985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 06:37:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.480468, cluster_1_dim_2=0.117222, cluster_1_dim_3=-0.064458, cluster_1_dim_4=-0.363091, cluster_1_dim_5=-0.587235, cluster_2_dim_1=-0.480468, cluster_2_dim_2=0.596450, cluster_2_dim_3=0.861639, cluster_2_dim_4=-0.396485, cluster_2_dim_5=-0.133140, cluster_3_dim_1=0.093504, cluster_3_dim_2=-0.311085, cluster_3_dim_3=-0.570943, cluster_3_dim_4=0.267231, cluster_3_dim_5=0.543808, cluster_4_dim_1=0.582963, cluster_4_dim_2=0.853743, cluster_4_dim_3=-0.529514, cluster_4_dim_4=-0.925581, cluster_4_dim_5=0.664433, cluster_5_dim_1=0.582963, cluster_5_dim_2=0.554241, cluster_5_dim_3=0.505835, cluster_5_dim_4=0.307723, cluster_5_dim_5=0.119407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.431609, d2=0.289781, d3=0.621576, d4=0.603461, d5=0.603141, d6=0.535130, d7=0.483140, d8=0.298779, d9=0.397892, d10=0.277859, d11=0.829223, d12=0.295198, d13=0.222211, d14=0.448797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 07:08:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.464479, cluster_1_dim_2=-0.604444, cluster_1_dim_3=-0.288663, cluster_1_dim_4=-0.207101, cluster_1_dim_5=-0.163442, cluster_2_dim_1=-0.464479, cluster_2_dim_2=0.646714, cluster_2_dim_3=0.598294, cluster_2_dim_4=-0.379994, cluster_2_dim_5=-0.280810, cluster_3_dim_1=0.487353, cluster_3_dim_2=0.554241, cluster_3_dim_3=0.505835, cluster_3_dim_4=0.307723, cluster_3_dim_5=0.119407, cluster_4_dim_1=0.487353, cluster_4_dim_2=-0.143714, cluster_4_dim_3=-0.536338, cluster_4_dim_4=0.410118, cluster_4_dim_5=0.753828, cluster_5_dim_1=0.619351, cluster_5_dim_2=0.853743, cluster_5_dim_3=-0.529514, cluster_5_dim_4=-0.925581, cluster_5_dim_5=0.664433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.439298, d2=0.462065, d3=0.804987, d4=0.249693, d5=0.337662, d6=0.876181, d7=0.336886, d8=0.286995, d9=0.419886, d10=0.286995, d11=0.772600, d12=0.187667, d13=0.167745, d14=0.496228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 07:38:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim3_clusters5_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.546410, cluster_1_dim_2=0.506090, cluster_1_dim_3=-0.584802, cluster_2_dim_1=-0.229335, cluster_2_dim_2=-0.786286, cluster_2_dim_3=-0.539516, cluster_3_dim_1=-0.050386, cluster_3_dim_2=-0.030958, cluster_3_dim_3=0.838302, cluster_4_dim_1=0.442770, cluster_4_dim_2=-0.922402, cluster_4_dim_3=0.327853, cluster_5_dim_1=0.729602, cluster_5_dim_2=0.349444, cluster_5_dim_3=-0.096689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.017453, d2=0.043366, d3=0.039294, d4=0.060612, d5=0.417988, d6=0.185070, d7=0.337644, d8=0.440133, d9=0.308520, d10=0.108424, d11=0.043828, d12=0.038473, d13=0.272582, d14=0.038614, d15=0.608438, d16=0.143767, d17=0.039301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 08:08:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.531865, cluster_1_dim_2=-0.786195, cluster_1_dim_3=-0.539442, cluster_2_dim_1=-0.531865, cluster_2_dim_2=0.432763, cluster_2_dim_3=-0.573053, cluster_3_dim_1=0.395997, cluster_3_dim_2=0.419009, cluster_3_dim_3=-0.371370, cluster_4_dim_1=0.395997, cluster_4_dim_2=-0.371096, cluster_4_dim_3=0.546743, cluster_5_dim_1=0.850441, cluster_5_dim_2=0.889103, cluster_5_dim_3=-0.044852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.230919, d2=0.587475, d3=0.192737, d4=0.295211, d5=0.451227, d6=0.147379, d7=0.288250, d8=0.413381, d9=-0.000000, d10=0.081745, d11=0.299098, d12=0.364283, d13=0.073430, d14=0.421302, d15=0.627236, d16=0.205062, d17=0.068839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 08:38:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.546849, cluster_1_dim_2=0.505923, cluster_1_dim_3=-0.585342, cluster_2_dim_1=-0.139585, cluster_2_dim_2=-0.030687, cluster_2_dim_3=0.838452, cluster_3_dim_1=-0.139585, cluster_3_dim_2=-0.786195, cluster_3_dim_3=-0.539442, cluster_4_dim_1=0.647257, cluster_4_dim_2=0.348930, cluster_4_dim_3=-0.096564, cluster_5_dim_1=0.647257, cluster_5_dim_2=-0.922670, cluster_5_dim_3=0.328043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.015533, d2=0.020637, d3=0.028971, d4=0.094658, d5=0.418509, d6=0.184735, d7=0.338065, d8=0.439241, d9=0.335744, d10=0.108406, d11=0.082689, d12=0.137432, d13=0.246276, d14=0.023317, d15=0.609262, d16=0.143670, d17=0.065757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 09:08:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.547167, cluster_1_dim_2=0.505300, cluster_1_dim_3=-0.585167, cluster_2_dim_1=-0.229300, cluster_2_dim_2=-0.785565, cluster_2_dim_3=-0.538948, cluster_3_dim_1=-0.049308, cluster_3_dim_2=-0.031339, cluster_3_dim_3=0.837855, cluster_4_dim_1=0.442291, cluster_4_dim_2=-0.922560, cluster_4_dim_3=0.327693, cluster_5_dim_1=0.729079, cluster_5_dim_2=0.348674, cluster_5_dim_3=-0.096168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.017175, d2=0.043748, d3=0.039221, d4=0.060783, d5=0.419324, d6=0.184140, d7=0.336630, d8=0.438693, d9=0.309425, d10=0.108349, d11=0.043448, d12=0.038320, d13=0.272796, d14=0.038768, d15=0.609203, d16=0.144114, d17=0.039375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 09:38:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim4_clusters4_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.711682, cluster_1_dim_2=-0.531117, cluster_1_dim_3=-0.506520, cluster_1_dim_4=0.274840, cluster_2_dim_1=-0.261093, cluster_2_dim_2=0.501852, cluster_2_dim_3=-0.629586, cluster_2_dim_4=0.231972, cluster_3_dim_1=-0.090869, cluster_3_dim_2=0.676509, cluster_3_dim_3=0.620230, cluster_3_dim_4=-0.270316, cluster_4_dim_1=0.529638, cluster_4_dim_2=-0.546330, cluster_4_dim_3=0.260019, cluster_4_dim_4=-0.087290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.131420, d2=0.672275, d3=0.399738, d4=0.883191, d5=1.077876, d6=0.393259, d7=0.740713, d8=0.023271, d9=0.466964, d10=0.502650, d11=0.235019, d12=0.270541, d13=0.301172, d14=0.309559, d15=0.437960, d16=0.635038, d17=0.918412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 10:08:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.467726, cluster_1_dim_2=0.357413, cluster_1_dim_3=-0.680609, cluster_1_dim_4=0.302218, cluster_2_dim_1=-0.467726, cluster_2_dim_2=-0.771350, cluster_2_dim_3=-0.597286, cluster_2_dim_4=0.448807, cluster_3_dim_1=-0.194836, cluster_3_dim_2=0.593548, cluster_3_dim_3=0.080397, cluster_3_dim_4=-0.116782, cluster_4_dim_1=0.529907, cluster_4_dim_2=-0.546531, cluster_4_dim_3=0.259778, cluster_4_dim_4=-0.087253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.131378, d2=0.609328, d3=0.562754, d4=0.883202, d5=1.669256, d6=0.393431, d7=0.967745, d8=0.636298, d9=0.466728, d10=0.271784, d11=0.415642, d12=0.279424, d13=0.545229, d14=0.318050, d15=0.298309, d16=0.975489, d17=0.918511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 10:38:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.711901, cluster_1_dim_2=-0.530690, cluster_1_dim_3=-0.507425, cluster_1_dim_4=0.274531, cluster_2_dim_1=-0.204408, cluster_2_dim_2=0.676435, cluster_2_dim_3=0.620478, cluster_2_dim_4=-0.270721, cluster_3_dim_1=-0.204408, cluster_3_dim_2=0.501834, cluster_3_dim_3=-0.628964, cluster_3_dim_4=0.232394, cluster_4_dim_1=0.529907, cluster_4_dim_2=-0.546531, cluster_4_dim_3=0.259778, cluster_4_dim_4=-0.087253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.131378, d2=0.641331, d3=0.399385, d4=0.883202, d5=1.247600, d6=0.393431, d7=0.592905, d8=0.042928, d9=0.466728, d10=0.561477, d11=0.251604, d12=0.271018, d13=0.334702, d14=0.301438, d15=0.437832, d16=0.581340, d17=0.918511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 11:08:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.394974, cluster_1_dim_2=0.298535, cluster_1_dim_3=-0.613476, cluster_1_dim_4=0.272839, cluster_2_dim_1=-0.394974, cluster_2_dim_2=0.522715, cluster_2_dim_3=0.690082, cluster_2_dim_4=0.077055, cluster_3_dim_1=0.233052, cluster_3_dim_2=-0.715451, cluster_3_dim_3=0.111110, cluster_3_dim_4=0.095313, cluster_4_dim_1=0.729319, cluster_4_dim_2=0.429564, cluster_4_dim_3=0.418180, cluster_4_dim_4=-0.921926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.344336, d2=0.964581, d3=0.512191, d4=0.801777, d5=0.329478, d6=0.198588, d7=0.251149, d8=0.036330, d9=0.564860, d10=0.362605, d11=0.189417, d12=1.057803, d13=0.191387, d14=0.260046, d15=1.225246, d16=0.995867, d17=0.329478</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 11:38:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim4_clusters5_points16_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.865624, cluster_1_dim_2=-0.316171, cluster_1_dim_3=-0.156520, cluster_1_dim_4=-0.299286, cluster_2_dim_1=-0.804718, cluster_2_dim_2=0.806150, cluster_2_dim_3=0.501169, cluster_2_dim_4=0.882299, cluster_3_dim_1=-0.169069, cluster_3_dim_2=-0.273223, cluster_3_dim_3=0.654764, cluster_3_dim_4=0.255966, cluster_4_dim_1=0.221837, cluster_4_dim_2=0.602513, cluster_4_dim_3=0.473512, cluster_4_dim_4=-0.255707, cluster_5_dim_1=0.613053, cluster_5_dim_2=-0.491348, cluster_5_dim_3=-0.246585, cluster_5_dim_4=-0.689118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.954174, d2=0.663631, d3=0.298898, d4=0.476843, d5=0.138036, d6=0.463346, d7=0.164997, d8=0.134073, d9=0.498605, d10=0.353857, d11=0.367493, d12=0.496671, d13=0.000002, d14=0.094810, d15=0.429029, d16=0.220902</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 12:08:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.866132, cluster_1_dim_2=-0.315613, cluster_1_dim_3=-0.156455, cluster_1_dim_4=-0.299128, cluster_2_dim_1=-0.043185, cluster_2_dim_2=-0.877136, cluster_2_dim_3=-0.251401, cluster_2_dim_4=-0.680049, cluster_3_dim_1=-0.043185, cluster_3_dim_2=-0.273508, cluster_3_dim_3=0.655303, cluster_3_dim_4=0.255595, cluster_4_dim_1=-0.043185, cluster_4_dim_2=0.799765, cluster_4_dim_3=0.459772, cluster_4_dim_4=0.197196, cluster_5_dim_1=0.674766, cluster_5_dim_2=0.000645, cluster_5_dim_3=0.020300, cluster_5_dim_4=-0.623787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.961112, d2=0.663346, d3=0.363316, d4=0.156555, d5=0.406190, d6=0.479661, d7=0.692327, d8=0.152633, d9=0.338152, d10=0.354450, d11=0.367072, d12=0.496781, d13=1.049489, d14=0.054230, d15=0.498143, d16=0.063751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 12:38:39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.841706, cluster_1_dim_2=-0.231329, cluster_1_dim_3=-0.374003, cluster_1_dim_4=-0.312165, cluster_2_dim_1=-0.555370, cluster_2_dim_2=-0.644010, cluster_2_dim_3=0.669419, cluster_2_dim_4=0.237157, cluster_3_dim_1=-0.222291, cluster_3_dim_2=0.799765, cluster_3_dim_3=0.459772, cluster_3_dim_4=0.197196, cluster_4_dim_1=0.005577, cluster_4_dim_2=-0.040558, cluster_4_dim_3=0.580760, cluster_4_dim_4=-0.046812, cluster_5_dim_1=0.612883, cluster_5_dim_2=-0.491146, cluster_5_dim_3=-0.246594, cluster_5_dim_4=-0.689039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.954006, d2=0.345107, d3=0.521068, d4=0.476919, d5=0.504310, d6=0.430380, d7=0.165138, d8=0.380691, d9=0.498557, d10=0.491492, d11=0.382676, d12=0.430380, d13=0.809141, d14=0.060980, d15=0.235616, d16=0.109741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 13:08:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.866132, cluster_1_dim_2=-0.315613, cluster_1_dim_3=-0.156455, cluster_1_dim_4=-0.299128, cluster_2_dim_1=-0.160225, cluster_2_dim_2=-0.378530, cluster_2_dim_3=0.622792, cluster_2_dim_4=0.430283, cluster_3_dim_1=-0.160225, cluster_3_dim_2=0.799765, cluster_3_dim_3=0.459772, cluster_3_dim_4=0.197196, cluster_4_dim_1=0.232242, cluster_4_dim_2=-0.029431, cluster_4_dim_3=0.575039, cluster_4_dim_4=-0.521991, cluster_5_dim_1=0.633419, cluster_5_dim_2=-0.540828, cluster_5_dim_3=-0.471393, cluster_5_dim_4=-0.644651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.748518, d2=0.663346, d3=0.148607, d4=0.619635, d5=0.463044, d6=0.257200, d7=0.061725, d8=0.094526, d9=0.311347, d10=0.354450, d11=0.367072, d12=0.496781, d13=0.885165, d14=0.209481, d15=0.478083, d16=0.086540</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 13:38:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters3_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.450201, cluster_1_dim_2=-0.162434, cluster_1_dim_3=-0.393615, cluster_1_dim_4=-0.161394, cluster_1_dim_5=0.597843, cluster_2_dim_1=-0.227271, cluster_2_dim_2=-0.203994, cluster_2_dim_3=-0.145010, cluster_2_dim_4=0.404236, cluster_2_dim_5=-0.694370, cluster_3_dim_1=0.301365, cluster_3_dim_2=-0.272804, cluster_3_dim_3=0.332752, cluster_3_dim_4=0.863571, cluster_3_dim_5=0.532542</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.017006, d2=0.730399, d3=1.288069, d4=0.931842, d5=2.000763, d6=0.708358, d7=1.001211, d8=0.208219, d9=0.798503, d10=1.480851, d11=1.469094, d12=0.499580, d13=0.676125, d14=0.354010, d15=0.766486, d16=1.791168, d17=0.787102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 14:08:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.239524, cluster_1_dim_2=-0.133286, cluster_1_dim_3=-0.167960, cluster_1_dim_4=0.210645, cluster_1_dim_5=0.807282, cluster_2_dim_1=-0.088134, cluster_2_dim_2=-0.113126, cluster_2_dim_3=0.699074, cluster_2_dim_4=0.498436, cluster_2_dim_5=-0.309830, cluster_3_dim_1=-0.088134, cluster_3_dim_2=-0.362846, cluster_3_dim_3=-0.531427, cluster_3_dim_4=0.384440, cluster_3_dim_5=-0.388017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.022803, d2=2.083691, d3=1.149314, d4=1.444049, d5=1.685877, d6=0.397740, d7=0.831596, d8=0.260658, d9=0.767480, d10=0.940735, d11=2.282397, d12=0.552565, d13=0.641204, d14=0.750735, d15=0.830877, d16=2.112246, d17=1.113394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 14:38:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 15:08:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.343030, cluster_1_dim_2=0.140964, cluster_1_dim_3=0.027656, cluster_1_dim_4=0.208010, cluster_1_dim_5=0.705044, cluster_2_dim_1=-0.259367, cluster_2_dim_2=-0.293207, cluster_2_dim_3=-0.249647, cluster_2_dim_4=0.220819, cluster_2_dim_5=-0.620193, cluster_3_dim_1=0.552924, cluster_3_dim_2=-0.832295, cluster_3_dim_3=-0.004684, cluster_3_dim_4=0.924366, cluster_3_dim_5=0.496531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.117849, d2=0.073999, d3=1.492435, d4=1.663215, d5=2.291009, d6=0.311059, d7=0.950257, d8=0.274451, d9=1.219884, d10=1.524491, d11=0.466813, d12=0.314075, d13=0.585600, d14=0.527189, d15=0.913607, d16=2.126951, d17=0.754637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 15:38:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters4_points16_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.636870, cluster_1_dim_2=0.168304, cluster_1_dim_3=0.546836, cluster_1_dim_4=-0.620910, cluster_1_dim_5=-0.729885, cluster_2_dim_1=-0.179875, cluster_2_dim_2=-0.530621, cluster_2_dim_3=0.148116, cluster_2_dim_4=0.300879, cluster_2_dim_5=-0.237196, cluster_3_dim_1=0.154490, cluster_3_dim_2=0.412934, cluster_3_dim_3=0.296662, cluster_3_dim_4=-0.831467, cluster_3_dim_5=0.454562, cluster_4_dim_1=0.483764, cluster_4_dim_2=0.775003, cluster_4_dim_3=-0.224239, cluster_4_dim_4=0.423956, cluster_4_dim_5=-0.498483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.822239, d2=1.074739, d3=0.255996, d4=1.154727, d5=0.397081, d6=0.985136, d7=0.729798, d8=0.800248, d9=0.423194, d10=0.373580, d11=0.614480, d12=1.258765, d13=0.340394, d14=0.260513, d15=0.759592, d16=0.489449</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 16:09:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 16:39:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.395523, cluster_1_dim_2=0.248206, cluster_1_dim_3=-0.080298, cluster_1_dim_4=0.187059, cluster_1_dim_5=-0.743464, cluster_2_dim_1=0.099553, cluster_2_dim_2=0.587650, cluster_2_dim_3=0.192955, cluster_2_dim_4=-0.521956, cluster_2_dim_5=0.648100, cluster_3_dim_1=0.099553, cluster_3_dim_2=-0.709428, cluster_3_dim_3=0.301830, cluster_3_dim_4=0.072115, cluster_3_dim_5=-0.079405, cluster_4_dim_1=0.099553, cluster_4_dim_2=0.095103, cluster_4_dim_3=0.748779, cluster_4_dim_4=-0.761373, cluster_4_dim_5=-0.558707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.419820, d2=0.773154, d3=0.275593, d4=0.584441, d5=1.054214, d6=1.056443, d7=0.315876, d8=1.284595, d9=0.914964, d10=1.419741, d11=0.932311, d12=0.891072, d13=0.908113, d14=0.897855, d15=0.791953, d16=0.423854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 17:09:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.217607, cluster_1_dim_2=-0.505247, cluster_1_dim_3=0.282241, cluster_1_dim_4=0.148830, cluster_1_dim_5=-0.253601, cluster_2_dim_1=-0.217607, cluster_2_dim_2=0.470605, cluster_2_dim_3=0.279033, cluster_2_dim_4=-0.786825, cluster_2_dim_5=0.755623, cluster_3_dim_1=-0.217607, cluster_3_dim_2=0.322880, cluster_3_dim_3=0.396007, cluster_3_dim_4=-0.709405, cluster_3_dim_5=-0.758132, cluster_4_dim_1=0.483764, cluster_4_dim_2=0.775003, cluster_4_dim_3=-0.224239, cluster_4_dim_4=0.423956, cluster_4_dim_5=-0.498483</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.051514, d2=1.066511, d3=0.433673, d4=0.996752, d5=0.727188, d6=1.225421, d7=0.717108, d8=0.800248, d9=0.423194, d10=0.373580, d11=0.852426, d12=0.570109, d13=0.466199, d14=0.560104, d15=0.812550, d16=0.434348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 17:39:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters5_points15_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.553747, cluster_1_dim_2=-0.414507, cluster_1_dim_3=0.769259, cluster_1_dim_4=-0.313617, cluster_1_dim_5=0.452210, cluster_2_dim_1=-0.458682, cluster_2_dim_2=0.548365, cluster_2_dim_3=-0.422579, cluster_2_dim_4=0.667594, cluster_2_dim_5=-0.258714, cluster_3_dim_1=-0.384489, cluster_3_dim_2=-0.700164, cluster_3_dim_3=-0.476919, cluster_3_dim_4=-0.395659, cluster_3_dim_5=-0.144714, cluster_4_dim_1=-0.214284, cluster_4_dim_2=0.473694, cluster_4_dim_3=0.792389, cluster_4_dim_4=0.293153, cluster_4_dim_5=-0.250594, cluster_5_dim_1=0.489762, cluster_5_dim_2=0.289839, cluster_5_dim_3=-0.267976, cluster_5_dim_4=-0.443692, cluster_5_dim_5=-0.164363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.459563, d2=0.392640, d3=0.224794, d4=0.380074, d5=0.240620, d6=0.200238, d7=0.548396, d8=0.000003, d9=0.510391, d10=0.427420, d11=0.624665, d12=0.457514, d13=0.281260, d14=0.380111, d15=0.432793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 18:09:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.373093, cluster_1_dim_2=-0.452714, cluster_1_dim_3=-0.425276, cluster_1_dim_4=-0.408157, cluster_1_dim_5=-0.149898, cluster_2_dim_1=-0.373093, cluster_2_dim_2=0.184102, cluster_2_dim_3=0.871206, cluster_2_dim_4=-0.134247, cluster_2_dim_5=-0.036347, cluster_3_dim_1=-0.373093, cluster_3_dim_2=0.288498, cluster_3_dim_3=-0.477143, cluster_3_dim_4=0.727431, cluster_3_dim_5=-0.276134, cluster_4_dim_1=-0.373093, cluster_4_dim_2=-0.722392, cluster_4_dim_3=0.588767, cluster_4_dim_4=-0.067677, cluster_4_dim_5=0.726349, cluster_5_dim_1=-0.373093, cluster_5_dim_2=0.720886, cluster_5_dim_3=-0.387373, cluster_5_dim_4=0.626828, cluster_5_dim_5=-0.246148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.396322, d2=0.229647, d3=0.186732, d4=0.619209, d5=0.231502, d6=0.211767, d7=0.211197, d8=1.321990, d9=0.482097, d10=0.709256, d11=0.823987, d12=0.232354, d13=0.323467, d14=0.827952, d15=0.454782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 18:39:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.546822, cluster_1_dim_2=0.547931, cluster_1_dim_3=-0.423281, cluster_1_dim_4=0.667069, cluster_1_dim_5=-0.258143, cluster_2_dim_1=-0.546822, cluster_2_dim_2=-0.370722, cluster_2_dim_3=0.395820, cluster_2_dim_4=-0.617819, cluster_2_dim_5=0.257513, cluster_3_dim_1=-0.456951, cluster_3_dim_2=-0.491240, cluster_3_dim_3=0.705530, cluster_3_dim_4=-0.186032, cluster_3_dim_5=0.559595, cluster_4_dim_1=-0.079557, cluster_4_dim_2=-0.417168, cluster_4_dim_3=-0.510709, cluster_4_dim_4=-0.365501, cluster_4_dim_5=-0.328561, cluster_5_dim_1=-0.079557, cluster_5_dim_2=0.473717, cluster_5_dim_3=0.792577, cluster_5_dim_4=0.292632, cluster_5_dim_5=-0.250206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.427719, d2=0.386840, d3=0.192042, d4=0.374749, d5=0.443200, d6=0.238986, d7=0.366723, d8=0.916198, d9=0.398708, d10=0.465193, d11=0.624369, d12=0.295222, d13=0.351677, d14=0.421319, d15=0.517519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 19:09:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.453750, cluster_1_dim_2=0.317133, cluster_1_dim_3=0.472615, cluster_1_dim_4=0.410297, cluster_1_dim_5=-0.305386, cluster_2_dim_1=-0.453750, cluster_2_dim_2=-0.413953, cluster_2_dim_3=0.769301, cluster_2_dim_4=-0.314402, cluster_2_dim_5=0.451930, cluster_3_dim_1=-0.383902, cluster_3_dim_2=-0.700402, cluster_3_dim_3=-0.477358, cluster_3_dim_4=-0.396261, cluster_3_dim_5=-0.145419, cluster_4_dim_1=-0.253688, cluster_4_dim_2=0.290351, cluster_4_dim_3=-0.269027, cluster_4_dim_4=-0.443846, cluster_4_dim_5=-0.163336, cluster_5_dim_1=-0.253688, cluster_5_dim_2=0.683922, cluster_5_dim_3=-0.487274, cluster_5_dim_4=0.672430, cluster_5_dim_5=-0.218741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.549843, d2=0.581886, d3=0.318231, d4=0.400752, d5=0.248050, d6=0.128299, d7=0.504888, d8=0.552252, d9=0.511669, d10=0.494105, d11=0.624458, d12=0.466570, d13=0.209339, d14=0.762431, d15=0.431717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 19:39:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim4_clusters5_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.597768, cluster_1_dim_2=0.081365, cluster_1_dim_3=-0.599423, cluster_1_dim_4=-0.835238, cluster_2_dim_1=-0.597769, cluster_2_dim_2=0.551823, cluster_2_dim_3=-0.076007, cluster_2_dim_4=0.070204, cluster_3_dim_1=-0.213907, cluster_3_dim_2=-0.682392, cluster_3_dim_3=0.375659, cluster_3_dim_4=0.449184, cluster_4_dim_1=0.521755, cluster_4_dim_2=0.142369, cluster_4_dim_3=-0.493149, cluster_4_dim_4=0.849573, cluster_5_dim_1=0.521755, cluster_5_dim_2=0.598796, cluster_5_dim_3=0.133998, cluster_5_dim_4=-0.604727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.073233, d2=0.203034, d3=0.181200, d4=0.622324, d5=0.195754, d6=0.335553, d7=0.370719, d8=0.368823, d9=0.373270, d10=0.542030, d11=0.440306, d12=0.544998, d13=0.216054, d14=0.751977, d15=0.589470, d16=0.336900, d17=0.063318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 20:09:37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.608029, cluster_1_dim_2=0.601444, cluster_1_dim_3=-0.147511, cluster_1_dim_4=-0.530505, cluster_2_dim_1=-0.016386, cluster_2_dim_2=0.553344, cluster_2_dim_3=-0.190748, cluster_2_dim_4=-0.629143, cluster_3_dim_1=-0.016386, cluster_3_dim_2=0.106956, cluster_3_dim_3=0.100097, cluster_3_dim_4=0.044886, cluster_4_dim_1=-0.016386, cluster_4_dim_2=-0.025849, cluster_4_dim_3=-0.375528, cluster_4_dim_4=0.806664, cluster_5_dim_1=-0.016386, cluster_5_dim_2=-0.646329, cluster_5_dim_3=0.544829, cluster_5_dim_4=0.376112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.249382, d2=0.586656, d3=0.174926, d4=0.589934, d5=0.969237, d6=0.223787, d7=0.524609, d8=0.489546, d9=1.085559, d10=0.680821, d11=0.434417, d12=0.554891, d13=0.596895, d14=0.518568, d15=0.652547, d16=0.682648, d17=0.230868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 20:39:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.792752, cluster_1_dim_2=0.771610, cluster_1_dim_3=-0.052194, cluster_1_dim_4=-0.202108, cluster_2_dim_1=-0.213907, cluster_2_dim_2=-0.682392, cluster_2_dim_3=0.375659, cluster_2_dim_4=0.449184, cluster_3_dim_1=-0.108617, cluster_3_dim_2=0.182255, cluster_3_dim_3=-0.302437, cluster_3_dim_4=0.664122, cluster_4_dim_1=-0.108617, cluster_4_dim_2=0.279612, cluster_4_dim_3=-0.294338, cluster_4_dim_4=-0.879060, cluster_5_dim_1=0.781486, cluster_5_dim_2=0.560141, cluster_5_dim_3=0.043081, cluster_5_dim_4=-0.423739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.073233, d2=0.840920, d3=0.079410, d4=0.622324, d5=0.703059, d6=0.475068, d7=0.112492, d8=0.204984, d9=0.296811, d10=0.537615, d11=0.296811, d12=0.306518, d13=0.631619, d14=0.751977, d15=0.589470, d16=0.213781, d17=0.063318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 21:09:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.680293, cluster_1_dim_2=0.551823, cluster_1_dim_3=-0.076007, cluster_1_dim_4=0.070204, cluster_2_dim_1=-0.290349, cluster_2_dim_2=0.279612, cluster_2_dim_3=-0.294338, cluster_2_dim_4=-0.879060, cluster_3_dim_1=-0.213907, cluster_3_dim_2=-0.682392, cluster_3_dim_3=0.375659, cluster_3_dim_4=0.449184, cluster_4_dim_1=0.674227, cluster_4_dim_2=0.560141, cluster_4_dim_3=0.043081, cluster_4_dim_4=-0.423739, cluster_5_dim_1=0.674227, cluster_5_dim_2=0.142369, cluster_5_dim_3=-0.493149, cluster_5_dim_4=0.849573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.073233, d2=0.234449, d3=0.146293, d4=0.622324, d5=0.557059, d6=0.367188, d7=0.371310, d8=0.211433, d9=0.344418, d10=0.578087, d11=0.272214, d12=0.555426, d13=0.203560, d14=0.751977, d15=0.589470, d16=0.295102, d17=0.063318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 21:39:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters4_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.547660, cluster_1_dim_2=-0.549574, cluster_1_dim_3=0.117407, cluster_1_dim_4=-0.584656, cluster_1_dim_5=0.372085, cluster_2_dim_1=-0.421946, cluster_2_dim_2=0.536133, cluster_2_dim_3=-0.731257, cluster_2_dim_4=0.375978, cluster_2_dim_5=0.146319, cluster_3_dim_1=-0.183795, cluster_3_dim_2=0.551647, cluster_3_dim_3=0.429123, cluster_3_dim_4=-0.175049, cluster_3_dim_5=-0.327354, cluster_4_dim_1=0.077417, cluster_4_dim_2=-0.562330, cluster_4_dim_3=0.015528, cluster_4_dim_4=0.561016, cluster_4_dim_5=-0.222412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.374971, d2=0.755239, d3=0.740567, d4=0.653453, d5=0.456916, d6=0.607459, d7=0.511671, d8=0.796694, d9=1.380258, d10=0.925229, d11=0.626241, d12=1.453711, d13=0.684383, d14=0.877259, d15=0.309544, d16=0.604060, d17=0.459975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 22:09:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.855581, cluster_1_dim_2=-0.795495, cluster_1_dim_3=0.078809, cluster_1_dim_4=-0.927058, cluster_1_dim_5=0.799746, cluster_2_dim_1=-0.483181, cluster_2_dim_2=-0.321758, cluster_2_dim_3=-0.722905, cluster_2_dim_4=-0.124956, cluster_2_dim_5=-0.424672, cluster_3_dim_1=-0.081715, cluster_3_dim_2=-0.095251, cluster_3_dim_3=-0.035517, cluster_3_dim_4=0.567343, cluster_3_dim_5=0.047793, cluster_4_dim_1=-0.081715, cluster_4_dim_2=0.373276, cluster_4_dim_3=0.553295, cluster_4_dim_4=-0.274695, cluster_4_dim_5=-0.264873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.708102, d2=0.445034, d3=0.751315, d4=0.720479, d5=-0.000000, d6=0.464804, d7=0.588960, d8=1.220615, d9=1.044641, d10=0.627472, d11=1.746106, d12=2.246294, d13=1.202036, d14=0.753946, d15=0.895315, d16=0.879098, d17=0.377170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 22:39:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.485097, cluster_1_dim_2=0.536706, cluster_1_dim_3=-0.731729, cluster_1_dim_4=0.375861, cluster_1_dim_5=0.146671, cluster_2_dim_1=-0.485097, cluster_2_dim_2=-0.549911, cluster_2_dim_3=0.117057, cluster_2_dim_4=-0.584914, cluster_2_dim_5=0.371925, cluster_3_dim_1=-0.041530, cluster_3_dim_2=-0.562301, cluster_3_dim_3=0.014787, cluster_3_dim_4=0.561310, cluster_3_dim_5=-0.222373, cluster_4_dim_1=-0.041530, cluster_4_dim_2=0.551406, cluster_4_dim_3=0.429545, cluster_4_dim_4=-0.175473, cluster_4_dim_5=-0.327568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.375710, d2=0.741382, d3=0.740722, d4=0.748112, d5=0.499126, d6=0.640868, d7=0.584357, d8=0.780199, d9=1.235715, d10=0.706845, d11=0.582120, d12=1.578542, d13=0.722742, d14=0.911750, d15=0.365368, d16=0.817516, d17=0.397099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 23:10:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.333402, cluster_1_dim_2=-0.134686, cluster_1_dim_3=0.561543, cluster_1_dim_4=-0.583016, cluster_1_dim_5=0.072572, cluster_2_dim_1=-0.333402, cluster_2_dim_2=0.524344, cluster_2_dim_3=-0.199200, cluster_2_dim_4=0.285852, cluster_2_dim_5=-0.116133, cluster_3_dim_1=0.050002, cluster_3_dim_2=-0.726840, cluster_3_dim_3=0.620092, cluster_3_dim_4=0.887530, cluster_3_dim_5=0.300374, cluster_4_dim_1=0.050002, cluster_4_dim_2=-0.583594, cluster_4_dim_3=-0.424881, cluster_4_dim_4=0.104845, cluster_4_dim_5=-0.373598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.749159, d2=0.919693, d3=0.914704, d4=0.678694, d5=1.589518, d6=0.737018, d7=0.248428, d8=0.446175, d9=0.982998, d10=1.429493, d11=1.414729, d12=0.521191, d13=0.532655, d14=0.296218, d15=0.453308, d16=0.815768, d17=0.607343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-08 23:40:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters5_points16_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.621683, cluster_1_dim_2=0.387920, cluster_1_dim_3=0.660493, cluster_1_dim_4=0.745458, cluster_1_dim_5=0.450154, cluster_2_dim_1=-0.621683, cluster_2_dim_2=0.006168, cluster_2_dim_3=-0.358398, cluster_2_dim_4=-0.762481, cluster_2_dim_5=-0.445842, cluster_3_dim_1=-0.218741, cluster_3_dim_2=-0.653458, cluster_3_dim_3=-0.301268, cluster_3_dim_4=0.107120, cluster_3_dim_5=-0.112442, cluster_4_dim_1=0.154485, cluster_4_dim_2=0.740089, cluster_4_dim_3=0.117174, cluster_4_dim_4=-0.090870, cluster_4_dim_5=0.686184, cluster_5_dim_1=0.768284, cluster_5_dim_2=0.577365, cluster_5_dim_3=0.488462, cluster_5_dim_4=0.124489, cluster_5_dim_5=-0.616901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.552981, d2=0.207234, d3=0.561208, d4=0.220188, d5=0.202896, d6=0.406669, d7=0.368563, d8=0.603411, d9=0.367935, d10=0.226732, d11=0.829972, d12=0.738098, d13=0.655520, d14=0.395692, d15=0.123889, d16=0.671886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 00:10:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.296723, cluster_1_dim_2=0.131590, cluster_1_dim_3=0.384032, cluster_1_dim_4=0.438398, cluster_1_dim_5=0.418344, cluster_2_dim_1=-0.141575, cluster_2_dim_2=0.161336, cluster_2_dim_3=0.548811, cluster_2_dim_4=0.181710, cluster_2_dim_5=-0.791437, cluster_3_dim_1=-0.141575, cluster_3_dim_2=0.661287, cluster_3_dim_3=0.545977, cluster_3_dim_4=0.352690, cluster_3_dim_5=0.753178, cluster_4_dim_1=-0.141575, cluster_4_dim_2=-0.157643, cluster_4_dim_3=-0.480237, cluster_4_dim_4=-0.589674, cluster_4_dim_5=-0.356324, cluster_5_dim_1=0.822045, cluster_5_dim_2=0.751179, cluster_5_dim_3=-0.356555, cluster_5_dim_4=-0.096172, cluster_5_dim_5=0.280659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.738589, d2=0.287575, d3=0.200105, d4=0.896634, d5=0.776599, d6=1.176817, d7=0.330484, d8=0.979732, d9=0.616828, d10=0.484684, d11=0.452787, d12=1.502726, d13=0.948734, d14=1.185786, d15=0.632610, d16=0.452787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 00:40:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.731857, cluster_1_dim_2=0.006318, cluster_1_dim_3=-0.358872, cluster_1_dim_4=-0.762901, cluster_1_dim_5=-0.445282, cluster_2_dim_1=-0.433145, cluster_2_dim_2=0.350403, cluster_2_dim_3=0.579135, cluster_2_dim_4=0.673649, cluster_2_dim_5=0.468150, cluster_3_dim_1=-0.219094, cluster_3_dim_2=-0.655816, cluster_3_dim_3=-0.300929, cluster_3_dim_4=0.107575, cluster_3_dim_5=-0.110822, cluster_4_dim_1=0.289343, cluster_4_dim_2=0.875638, cluster_4_dim_3=0.104156, cluster_4_dim_4=-0.234617, cluster_4_dim_5=0.734038, cluster_5_dim_1=0.768332, cluster_5_dim_2=0.577045, cluster_5_dim_3=0.487697, cluster_5_dim_4=0.124170, cluster_5_dim_5=-0.616849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.668367, d2=0.076156, d3=0.505556, d4=0.331375, d5=0.202675, d6=0.406980, d7=0.370315, d8=0.596786, d9=0.504783, d10=0.202675, d11=0.588818, d12=0.734012, d13=0.657828, d14=0.396414, d15=0.074807, d16=0.670850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 01:10:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.731857, cluster_1_dim_2=0.006318, cluster_1_dim_3=-0.358872, cluster_1_dim_4=-0.762901, cluster_1_dim_5=-0.445282, cluster_2_dim_1=-0.470566, cluster_2_dim_2=0.250997, cluster_2_dim_3=0.560956, cluster_2_dim_4=0.611050, cluster_2_dim_5=0.615691, cluster_3_dim_1=-0.219094, cluster_3_dim_2=-0.655816, cluster_3_dim_3=-0.300929, cluster_3_dim_4=0.107575, cluster_3_dim_5=-0.110822, cluster_4_dim_1=0.412795, cluster_4_dim_2=0.619791, cluster_4_dim_3=0.528735, cluster_4_dim_4=0.324138, cluster_4_dim_5=-0.493139, cluster_5_dim_1=0.412795, cluster_5_dim_2=0.875638, cluster_5_dim_3=0.104156, cluster_5_dim_4=-0.234617, cluster_5_dim_5=0.734038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.548117, d2=0.096066, d3=0.483583, d4=0.422856, d5=0.202675, d6=0.661860, d7=0.370315, d8=1.013998, d9=0.477900, d10=0.202675, d11=0.490764, d12=0.734012, d13=0.657828, d14=0.483611, d15=0.127101, d16=0.884402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 01:40:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_gams_gurobi_no_mode_2025-07-01_21-08-08_dim5_clusters5_points17_1.pkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.474395, cluster_1_dim_2=0.250675, cluster_1_dim_3=-0.430617, cluster_1_dim_4=0.919695, cluster_1_dim_5=-0.861424, cluster_2_dim_1=-0.444825, cluster_2_dim_2=0.283435, cluster_2_dim_3=0.711028, cluster_2_dim_4=0.058112, cluster_2_dim_5=-0.245846, cluster_3_dim_1=0.304887, cluster_3_dim_2=-0.130907, cluster_3_dim_3=0.061684, cluster_3_dim_4=0.584246, cluster_3_dim_5=0.640512, cluster_4_dim_1=0.304887, cluster_4_dim_2=0.497347, cluster_4_dim_3=0.353144, cluster_4_dim_4=-0.874107, cluster_4_dim_5=0.576492, cluster_5_dim_1=0.304887, cluster_5_dim_2=-0.894049, cluster_5_dim_3=-0.164336, cluster_5_dim_4=-0.644156, cluster_5_dim_5=-0.513044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=1.043879, d2=0.266532, d3=0.723394, d4=0.450657, d5=1.337626, d6=1.029810, d7=0.717493, d8=0.309448, d9=0.999422, d10=0.746635, d11=0.450657, d12=0.533123, d13=1.043398, d14=0.545567, d15=0.109757, d16=0.847168, d17=0.209876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 02:10:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.050671, cluster_1_dim_2=0.389518, cluster_1_dim_3=0.201500, cluster_1_dim_4=-0.372212, cluster_1_dim_5=0.515419, cluster_2_dim_1=-0.050671, cluster_2_dim_2=-0.442025, cluster_2_dim_3=0.680085, cluster_2_dim_4=0.663335, cluster_2_dim_5=0.232380, cluster_3_dim_1=-0.050671, cluster_3_dim_2=0.570798, cluster_3_dim_3=0.817922, cluster_3_dim_4=0.175497, cluster_3_dim_5=-0.289554, cluster_4_dim_1=-0.050671, cluster_4_dim_2=-0.025074, cluster_4_dim_3=-0.597638, cluster_4_dim_4=0.882509, cluster_4_dim_5=-0.334035, cluster_5_dim_1=0.195114, cluster_5_dim_2=-0.894049, cluster_5_dim_3=-0.164336, cluster_5_dim_4=-0.644156, cluster_5_dim_5=-0.513044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.461311, d2=0.799903, d3=0.494692, d4=0.672450, d5=1.535962, d6=0.557174, d7=0.737433, d8=0.289750, d9=0.777777, d10=0.855454, d11=1.354860, d12=0.809686, d13=1.181305, d14=1.548256, d15=0.355136, d16=1.187876, d17=0.173485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 02:40:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.555594, cluster_1_dim_2=0.177859, cluster_1_dim_3=0.096443, cluster_1_dim_4=-0.698033, cluster_1_dim_5=0.353747, cluster_2_dim_1=-0.555594, cluster_2_dim_2=-0.022640, cluster_2_dim_3=-0.027104, cluster_2_dim_4=0.743649, cluster_2_dim_5=-0.717128, cluster_3_dim_1=0.221160, cluster_3_dim_2=-0.130907, cluster_3_dim_3=0.061684, cluster_3_dim_4=0.584246, cluster_3_dim_5=0.640512, cluster_4_dim_1=0.221160, cluster_4_dim_2=-0.894049, cluster_4_dim_3=-0.164336, cluster_4_dim_4=-0.644156, cluster_4_dim_5=-0.513044, cluster_5_dim_1=0.221160, cluster_5_dim_2=0.656356, cluster_5_dim_3=0.822154, cluster_5_dim_4=-0.113287, cluster_5_dim_5=-0.088800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.513669, d2=0.273235, d3=0.149654, d4=0.429248, d5=1.292840, d6=0.152852, d7=0.730521, d8=0.292243, d9=1.034118, d10=1.459075, d11=1.063928, d12=0.608290, d13=1.246077, d14=1.371311, d15=0.704827, d16=0.937004, d17=0.179939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-07-09 03:10:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster_1_dim_1=-0.474395, cluster_1_dim_2=0.250675, cluster_1_dim_3=-0.430617, cluster_1_dim_4=0.919695, cluster_1_dim_5=-0.861424, cluster_2_dim_1=-0.333651, cluster_2_dim_2=0.542031, cluster_2_dim_3=0.508422, cluster_2_dim_4=-0.452814, cluster_2_dim_5=0.102407, cluster_3_dim_1=0.149309, cluster_3_dim_2=-0.209283, cluster_3_dim_3=-0.581028, cluster_3_dim_4=0.547267, cluster_3_dim_5=0.633076, cluster_4_dim_1=0.195114, cluster_4_dim_2=-0.894049, cluster_4_dim_3=-0.164336, cluster_4_dim_4=-0.644156, cluster_4_dim_5=-0.513044, cluster_5_dim_1=0.321807, cluster_5_dim_2=-0.106851, cluster_5_dim_3=0.637958, cluster_5_dim_4=0.526622, cluster_5_dim_5=0.269625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1=0.455772, d2=0.357231, d3=0.166028, d4=0.450657, d5=0.357231, d6=1.026165, d7=0.737433, d8=0.289750, d9=0.812946, d10=1.306793, d11=0.450657, d12=0.295625, d13=2.120913, d14=1.676699, d15=0.389293, d16=1.187039, d17=0.173485</t>
   </si>
 </sst>
 </file>
@@ -3483,6 +3972,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.3"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -26128,6 +26621,3526 @@
         <v>1</v>
       </c>
     </row>
+    <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B334" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C334" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D334" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E334" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F334" s="0" t="n">
+        <v>1801.38192462921</v>
+      </c>
+      <c r="G334" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H334" s="0" t="n">
+        <v>16.4611784207367</v>
+      </c>
+      <c r="I334" s="0" t="n">
+        <v>8.54746807520197</v>
+      </c>
+      <c r="J334" s="0" t="n">
+        <v>7.91371034553474</v>
+      </c>
+      <c r="K334" s="0" t="n">
+        <v>0.92585433205584</v>
+      </c>
+      <c r="L334" s="0" t="n">
+        <v>8.54746807520197</v>
+      </c>
+      <c r="M334" s="0" t="n">
+        <v>48.0749928301947</v>
+      </c>
+      <c r="P334" s="0" t="s">
+        <v>1057</v>
+      </c>
+      <c r="Q334" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R334" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S334" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T334" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U334" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V334" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W334" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X334" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B335" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C335" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D335" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E335" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F335" s="0" t="n">
+        <v>1802.08338570595</v>
+      </c>
+      <c r="G335" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H335" s="0" t="n">
+        <v>17.2190827399743</v>
+      </c>
+      <c r="I335" s="0" t="n">
+        <v>7.75561005153041</v>
+      </c>
+      <c r="J335" s="0" t="n">
+        <v>9.4634726884439</v>
+      </c>
+      <c r="K335" s="0" t="n">
+        <v>1.22020996743854</v>
+      </c>
+      <c r="L335" s="0" t="n">
+        <v>7.75561005153041</v>
+      </c>
+      <c r="M335" s="0" t="n">
+        <v>54.959214909133</v>
+      </c>
+      <c r="P335" s="0" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Q335" s="0" t="s">
+        <v>1061</v>
+      </c>
+      <c r="R335" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S335" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T335" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U335" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V335" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W335" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X335" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B336" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C336" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D336" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E336" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F336" s="0" t="n">
+        <v>1801.89191269875</v>
+      </c>
+      <c r="G336" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H336" s="0" t="n">
+        <v>16.5065831714553</v>
+      </c>
+      <c r="I336" s="0" t="n">
+        <v>7.58447413397988</v>
+      </c>
+      <c r="J336" s="0" t="n">
+        <v>8.92210903747542</v>
+      </c>
+      <c r="K336" s="0" t="n">
+        <v>1.17636488435008</v>
+      </c>
+      <c r="L336" s="0" t="n">
+        <v>7.58447413397988</v>
+      </c>
+      <c r="M336" s="0" t="n">
+        <v>54.0518225050012</v>
+      </c>
+      <c r="P336" s="0" t="s">
+        <v>1063</v>
+      </c>
+      <c r="Q336" s="0" t="s">
+        <v>1064</v>
+      </c>
+      <c r="R336" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S336" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T336" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U336" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V336" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W336" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X336" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E337" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F337" s="0" t="n">
+        <v>1801.94980931282</v>
+      </c>
+      <c r="G337" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H337" s="0" t="n">
+        <v>16.3984414859308</v>
+      </c>
+      <c r="I337" s="0" t="n">
+        <v>9.21056606457023</v>
+      </c>
+      <c r="J337" s="0" t="n">
+        <v>7.18787542136054</v>
+      </c>
+      <c r="K337" s="0" t="n">
+        <v>0.780394535034034</v>
+      </c>
+      <c r="L337" s="0" t="n">
+        <v>9.21056606457023</v>
+      </c>
+      <c r="M337" s="0" t="n">
+        <v>43.8326741448415</v>
+      </c>
+      <c r="P337" s="0" t="s">
+        <v>1066</v>
+      </c>
+      <c r="Q337" s="0" t="s">
+        <v>1067</v>
+      </c>
+      <c r="R337" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S337" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T337" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U337" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V337" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W337" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X337" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B338" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C338" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D338" s="0" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E338" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F338" s="0" t="n">
+        <v>1803.28591251373</v>
+      </c>
+      <c r="G338" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H338" s="0" t="n">
+        <v>10.0959630027843</v>
+      </c>
+      <c r="I338" s="0" t="n">
+        <v>6.03101777935141</v>
+      </c>
+      <c r="J338" s="0" t="n">
+        <v>4.06494522343291</v>
+      </c>
+      <c r="K338" s="0" t="n">
+        <v>0.674006506389385</v>
+      </c>
+      <c r="L338" s="0" t="n">
+        <v>6.03101777935141</v>
+      </c>
+      <c r="M338" s="0" t="n">
+        <v>40.2630756700659</v>
+      </c>
+      <c r="P338" s="0" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Q338" s="0" t="s">
+        <v>1071</v>
+      </c>
+      <c r="R338" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S338" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T338" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U338" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V338" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W338" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X338" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B339" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C339" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D339" s="0" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E339" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F339" s="0" t="n">
+        <v>1801.40095543861</v>
+      </c>
+      <c r="G339" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H339" s="0" t="n">
+        <v>11.1912830699943</v>
+      </c>
+      <c r="I339" s="0" t="n">
+        <v>7.46948371E-007</v>
+      </c>
+      <c r="J339" s="0" t="n">
+        <v>11.1912823230459</v>
+      </c>
+      <c r="K339" s="0" t="n">
+        <v>14982671.838568</v>
+      </c>
+      <c r="L339" s="0" t="n">
+        <v>7.46948371470952E-007</v>
+      </c>
+      <c r="M339" s="0" t="n">
+        <v>99.9999933256235</v>
+      </c>
+      <c r="P339" s="0" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Q339" s="0" t="s">
+        <v>1074</v>
+      </c>
+      <c r="R339" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S339" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T339" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U339" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V339" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W339" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X339" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A340" s="0" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B340" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C340" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D340" s="0" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E340" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F340" s="0" t="n">
+        <v>1803.8676981926</v>
+      </c>
+      <c r="G340" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H340" s="0" t="n">
+        <v>10.0959630028206</v>
+      </c>
+      <c r="I340" s="0" t="n">
+        <v>3.11337010837931</v>
+      </c>
+      <c r="J340" s="0" t="n">
+        <v>6.98259289444128</v>
+      </c>
+      <c r="K340" s="0" t="n">
+        <v>2.24277636495846</v>
+      </c>
+      <c r="L340" s="0" t="n">
+        <v>3.11337010837931</v>
+      </c>
+      <c r="M340" s="0" t="n">
+        <v>69.1622274417061</v>
+      </c>
+      <c r="P340" s="0" t="s">
+        <v>1070</v>
+      </c>
+      <c r="Q340" s="0" t="s">
+        <v>1071</v>
+      </c>
+      <c r="R340" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S340" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T340" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U340" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V340" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W340" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X340" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B341" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C341" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D341" s="0" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E341" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F341" s="0" t="n">
+        <v>1804.20830965042</v>
+      </c>
+      <c r="G341" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H341" s="0" t="n">
+        <v>10.3351893965194</v>
+      </c>
+      <c r="I341" s="0" t="n">
+        <v>4.67576194646575</v>
+      </c>
+      <c r="J341" s="0" t="n">
+        <v>5.65942745005363</v>
+      </c>
+      <c r="K341" s="0" t="n">
+        <v>1.21037544572418</v>
+      </c>
+      <c r="L341" s="0" t="n">
+        <v>4.67576194646575</v>
+      </c>
+      <c r="M341" s="0" t="n">
+        <v>54.7588170175147</v>
+      </c>
+      <c r="P341" s="0" t="s">
+        <v>1077</v>
+      </c>
+      <c r="Q341" s="0" t="s">
+        <v>1078</v>
+      </c>
+      <c r="R341" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S341" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T341" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U341" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V341" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W341" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X341" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D342" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E342" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F342" s="0" t="n">
+        <v>1808.81850814819</v>
+      </c>
+      <c r="G342" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H342" s="0" t="n">
+        <v>5.94056709950994</v>
+      </c>
+      <c r="I342" s="0" t="n">
+        <v>3.47662897344048</v>
+      </c>
+      <c r="J342" s="0" t="n">
+        <v>2.46393812606945</v>
+      </c>
+      <c r="K342" s="0" t="n">
+        <v>0.708714719025979</v>
+      </c>
+      <c r="L342" s="0" t="n">
+        <v>3.47662897344048</v>
+      </c>
+      <c r="M342" s="0" t="n">
+        <v>41.4764800194365</v>
+      </c>
+      <c r="P342" s="0" t="s">
+        <v>1081</v>
+      </c>
+      <c r="Q342" s="0" t="s">
+        <v>1082</v>
+      </c>
+      <c r="R342" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S342" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T342" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U342" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V342" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W342" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X342" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B343" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C343" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D343" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E343" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F343" s="0" t="n">
+        <v>1801.47929978371</v>
+      </c>
+      <c r="G343" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H343" s="0" t="n">
+        <v>8.99400162096597</v>
+      </c>
+      <c r="I343" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J343" s="0" t="n">
+        <v>8.99400162096597</v>
+      </c>
+      <c r="L343" s="0" t="n">
+        <v>2.77555756156289E-017</v>
+      </c>
+      <c r="M343" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P343" s="0" t="s">
+        <v>1084</v>
+      </c>
+      <c r="Q343" s="0" t="s">
+        <v>1085</v>
+      </c>
+      <c r="R343" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S343" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T343" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U343" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V343" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W343" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X343" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="0" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B344" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C344" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D344" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E344" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F344" s="0" t="n">
+        <v>1803.49917888641</v>
+      </c>
+      <c r="G344" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H344" s="0" t="n">
+        <v>6.33779627770983</v>
+      </c>
+      <c r="I344" s="0" t="n">
+        <v>1.4805680817625</v>
+      </c>
+      <c r="J344" s="0" t="n">
+        <v>4.85722819594734</v>
+      </c>
+      <c r="K344" s="0" t="n">
+        <v>3.28065170104518</v>
+      </c>
+      <c r="L344" s="0" t="n">
+        <v>1.48056808176249</v>
+      </c>
+      <c r="M344" s="0" t="n">
+        <v>76.6390711078915</v>
+      </c>
+      <c r="P344" s="0" t="s">
+        <v>1087</v>
+      </c>
+      <c r="Q344" s="0" t="s">
+        <v>1088</v>
+      </c>
+      <c r="R344" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S344" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T344" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U344" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V344" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W344" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X344" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B345" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C345" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D345" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E345" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F345" s="0" t="n">
+        <v>1804.19181203842</v>
+      </c>
+      <c r="G345" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H345" s="0" t="n">
+        <v>6.12488868903625</v>
+      </c>
+      <c r="I345" s="0" t="n">
+        <v>1.48277157236545</v>
+      </c>
+      <c r="J345" s="0" t="n">
+        <v>4.6421171166708</v>
+      </c>
+      <c r="K345" s="0" t="n">
+        <v>3.13070280222952</v>
+      </c>
+      <c r="L345" s="0" t="n">
+        <v>1.48277157236545</v>
+      </c>
+      <c r="M345" s="0" t="n">
+        <v>75.7910445781707</v>
+      </c>
+      <c r="P345" s="0" t="s">
+        <v>1090</v>
+      </c>
+      <c r="Q345" s="0" t="s">
+        <v>1091</v>
+      </c>
+      <c r="R345" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S345" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T345" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U345" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V345" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="W345" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X345" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D346" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E346" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F346" s="0" t="n">
+        <v>1802.63542985916</v>
+      </c>
+      <c r="G346" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H346" s="0" t="n">
+        <v>3.14350817939349</v>
+      </c>
+      <c r="I346" s="0" t="n">
+        <v>1.64907697256851</v>
+      </c>
+      <c r="J346" s="0" t="n">
+        <v>1.49443120682498</v>
+      </c>
+      <c r="K346" s="0" t="n">
+        <v>0.906222833551143</v>
+      </c>
+      <c r="L346" s="0" t="n">
+        <v>1.64907697256851</v>
+      </c>
+      <c r="M346" s="0" t="n">
+        <v>47.5402359892481</v>
+      </c>
+      <c r="P346" s="0" t="s">
+        <v>1094</v>
+      </c>
+      <c r="Q346" s="0" t="s">
+        <v>1095</v>
+      </c>
+      <c r="R346" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S346" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T346" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U346" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V346" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W346" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X346" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B347" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C347" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D347" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E347" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F347" s="0" t="n">
+        <v>1801.07713723183</v>
+      </c>
+      <c r="G347" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H347" s="0" t="n">
+        <v>4.74757593738402</v>
+      </c>
+      <c r="I347" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J347" s="0" t="n">
+        <v>4.74757593738402</v>
+      </c>
+      <c r="L347" s="0" t="n">
+        <v>2.22044604925031E-016</v>
+      </c>
+      <c r="M347" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P347" s="0" t="s">
+        <v>1097</v>
+      </c>
+      <c r="Q347" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="R347" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S347" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T347" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U347" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V347" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W347" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X347" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B348" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C348" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D348" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E348" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F348" s="0" t="n">
+        <v>1802.23565888405</v>
+      </c>
+      <c r="G348" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H348" s="0" t="n">
+        <v>3.29290080324997</v>
+      </c>
+      <c r="I348" s="0" t="n">
+        <v>1.13622684955207</v>
+      </c>
+      <c r="J348" s="0" t="n">
+        <v>2.1566739536979</v>
+      </c>
+      <c r="K348" s="0" t="n">
+        <v>1.89810155828311</v>
+      </c>
+      <c r="L348" s="0" t="n">
+        <v>1.13622684955207</v>
+      </c>
+      <c r="M348" s="0" t="n">
+        <v>65.4946529688761</v>
+      </c>
+      <c r="P348" s="0" t="s">
+        <v>1100</v>
+      </c>
+      <c r="Q348" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="R348" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S348" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T348" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U348" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V348" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W348" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X348" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="0" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B349" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C349" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D349" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E349" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F349" s="0" t="n">
+        <v>1802.28737568855</v>
+      </c>
+      <c r="G349" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H349" s="0" t="n">
+        <v>3.1435134627949</v>
+      </c>
+      <c r="I349" s="0" t="n">
+        <v>1.75221511329611</v>
+      </c>
+      <c r="J349" s="0" t="n">
+        <v>1.39129834949879</v>
+      </c>
+      <c r="K349" s="0" t="n">
+        <v>0.794022571167991</v>
+      </c>
+      <c r="L349" s="0" t="n">
+        <v>1.75221511329611</v>
+      </c>
+      <c r="M349" s="0" t="n">
+        <v>44.259341210576</v>
+      </c>
+      <c r="P349" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="Q349" s="0" t="s">
+        <v>1104</v>
+      </c>
+      <c r="R349" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S349" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T349" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U349" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V349" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W349" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X349" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B350" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C350" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D350" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E350" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F350" s="0" t="n">
+        <v>1802.75502705574</v>
+      </c>
+      <c r="G350" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H350" s="0" t="n">
+        <v>8.39905722960896</v>
+      </c>
+      <c r="I350" s="0" t="n">
+        <v>4.94290424771081</v>
+      </c>
+      <c r="J350" s="0" t="n">
+        <v>3.45615298189816</v>
+      </c>
+      <c r="K350" s="0" t="n">
+        <v>0.699215038102103</v>
+      </c>
+      <c r="L350" s="0" t="n">
+        <v>4.94290424771081</v>
+      </c>
+      <c r="M350" s="0" t="n">
+        <v>41.1492967295695</v>
+      </c>
+      <c r="P350" s="0" t="s">
+        <v>1107</v>
+      </c>
+      <c r="Q350" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="R350" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S350" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T350" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U350" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V350" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W350" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X350" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D351" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E351" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F351" s="0" t="n">
+        <v>1801.69073987007</v>
+      </c>
+      <c r="G351" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H351" s="0" t="n">
+        <v>10.3425566030789</v>
+      </c>
+      <c r="I351" s="0" t="n">
+        <v>0.356714387972044</v>
+      </c>
+      <c r="J351" s="0" t="n">
+        <v>9.98584221510684</v>
+      </c>
+      <c r="K351" s="0" t="n">
+        <v>27.9939429185274</v>
+      </c>
+      <c r="L351" s="0" t="n">
+        <v>0.356714387972044</v>
+      </c>
+      <c r="M351" s="0" t="n">
+        <v>96.5510037637517</v>
+      </c>
+      <c r="P351" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="Q351" s="0" t="s">
+        <v>1111</v>
+      </c>
+      <c r="R351" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S351" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T351" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U351" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V351" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W351" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X351" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B352" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C352" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D352" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E352" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F352" s="0" t="n">
+        <v>1802.65509176254</v>
+      </c>
+      <c r="G352" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H352" s="0" t="n">
+        <v>8.4568087663172</v>
+      </c>
+      <c r="I352" s="0" t="n">
+        <v>2.76843991353323</v>
+      </c>
+      <c r="J352" s="0" t="n">
+        <v>5.68836885278396</v>
+      </c>
+      <c r="K352" s="0" t="n">
+        <v>2.05471999770591</v>
+      </c>
+      <c r="L352" s="0" t="n">
+        <v>2.76843991353323</v>
+      </c>
+      <c r="M352" s="0" t="n">
+        <v>67.2637753787255</v>
+      </c>
+      <c r="P352" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="Q352" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="R352" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S352" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T352" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U352" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V352" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W352" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X352" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B353" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C353" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D353" s="0" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E353" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F353" s="0" t="n">
+        <v>1804.02435588837</v>
+      </c>
+      <c r="G353" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H353" s="0" t="n">
+        <v>8.61513930966357</v>
+      </c>
+      <c r="I353" s="0" t="n">
+        <v>3.61427609126115</v>
+      </c>
+      <c r="J353" s="0" t="n">
+        <v>5.00086321840241</v>
+      </c>
+      <c r="K353" s="0" t="n">
+        <v>1.3836417285591</v>
+      </c>
+      <c r="L353" s="0" t="n">
+        <v>3.61427609126115</v>
+      </c>
+      <c r="M353" s="0" t="n">
+        <v>58.0473865674229</v>
+      </c>
+      <c r="P353" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="Q353" s="0" t="s">
+        <v>1117</v>
+      </c>
+      <c r="R353" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S353" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T353" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U353" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V353" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W353" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X353" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B354" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C354" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D354" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E354" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F354" s="0" t="n">
+        <v>1807.63308429718</v>
+      </c>
+      <c r="G354" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H354" s="0" t="n">
+        <v>5.75536842489123</v>
+      </c>
+      <c r="I354" s="0" t="n">
+        <v>3.32857489474526</v>
+      </c>
+      <c r="J354" s="0" t="n">
+        <v>2.42679353014597</v>
+      </c>
+      <c r="K354" s="0" t="n">
+        <v>0.729078842112608</v>
+      </c>
+      <c r="L354" s="0" t="n">
+        <v>3.32857489474526</v>
+      </c>
+      <c r="M354" s="0" t="n">
+        <v>42.1657372906033</v>
+      </c>
+      <c r="P354" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="Q354" s="0" t="s">
+        <v>1121</v>
+      </c>
+      <c r="R354" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S354" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T354" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U354" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V354" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W354" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X354" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B355" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C355" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D355" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E355" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F355" s="0" t="n">
+        <v>1801.53207993507</v>
+      </c>
+      <c r="G355" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H355" s="0" t="n">
+        <v>7.09720701568754</v>
+      </c>
+      <c r="I355" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J355" s="0" t="n">
+        <v>7.09720701568754</v>
+      </c>
+      <c r="L355" s="0" t="n">
+        <v>1.11022302462516E-016</v>
+      </c>
+      <c r="M355" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P355" s="0" t="s">
+        <v>1123</v>
+      </c>
+      <c r="Q355" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="R355" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S355" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T355" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U355" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V355" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W355" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X355" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B356" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C356" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D356" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E356" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F356" s="0" t="n">
+        <v>1803.04927062988</v>
+      </c>
+      <c r="G356" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H356" s="0" t="n">
+        <v>6.79620074479402</v>
+      </c>
+      <c r="I356" s="0" t="n">
+        <v>0.677353454991945</v>
+      </c>
+      <c r="J356" s="0" t="n">
+        <v>6.11884728980208</v>
+      </c>
+      <c r="K356" s="0" t="n">
+        <v>9.03346287629823</v>
+      </c>
+      <c r="L356" s="0" t="n">
+        <v>0.677353454991945</v>
+      </c>
+      <c r="M356" s="0" t="n">
+        <v>90.0333512733448</v>
+      </c>
+      <c r="P356" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="Q356" s="0" t="s">
+        <v>1127</v>
+      </c>
+      <c r="R356" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S356" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T356" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U356" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V356" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W356" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X356" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B357" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C357" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D357" s="0" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E357" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F357" s="0" t="n">
+        <v>1804.3555855751</v>
+      </c>
+      <c r="G357" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H357" s="0" t="n">
+        <v>6.24551947989649</v>
+      </c>
+      <c r="I357" s="0" t="n">
+        <v>1.39370619762251</v>
+      </c>
+      <c r="J357" s="0" t="n">
+        <v>4.85181328227398</v>
+      </c>
+      <c r="K357" s="0" t="n">
+        <v>3.4812310446424</v>
+      </c>
+      <c r="L357" s="0" t="n">
+        <v>1.3937061976225</v>
+      </c>
+      <c r="M357" s="0" t="n">
+        <v>77.684703376418</v>
+      </c>
+      <c r="P357" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Q357" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="R357" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S357" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T357" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U357" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V357" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W357" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X357" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D358" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E358" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F358" s="0" t="n">
+        <v>1801.59959053993</v>
+      </c>
+      <c r="G358" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H358" s="0" t="n">
+        <v>16.5087856952192</v>
+      </c>
+      <c r="I358" s="0" t="n">
+        <v>10.0023433711413</v>
+      </c>
+      <c r="J358" s="0" t="n">
+        <v>6.50644232407786</v>
+      </c>
+      <c r="K358" s="0" t="n">
+        <v>0.650491798037069</v>
+      </c>
+      <c r="L358" s="0" t="n">
+        <v>10.0023433711413</v>
+      </c>
+      <c r="M358" s="0" t="n">
+        <v>39.4119982183916</v>
+      </c>
+      <c r="P358" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q358" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="R358" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S358" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T358" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U358" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V358" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W358" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X358" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B359" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C359" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D359" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E359" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F359" s="0" t="n">
+        <v>1801.82393145561</v>
+      </c>
+      <c r="G359" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H359" s="0" t="n">
+        <v>18.8673613166893</v>
+      </c>
+      <c r="I359" s="0" t="n">
+        <v>1.64472679097707</v>
+      </c>
+      <c r="J359" s="0" t="n">
+        <v>17.2226345257122</v>
+      </c>
+      <c r="K359" s="0" t="n">
+        <v>10.4714257834159</v>
+      </c>
+      <c r="L359" s="0" t="n">
+        <v>1.64472679097707</v>
+      </c>
+      <c r="M359" s="0" t="n">
+        <v>91.2826877941739</v>
+      </c>
+      <c r="P359" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Q359" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="R359" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S359" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T359" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U359" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V359" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W359" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X359" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B360" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C360" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D360" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E360" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F360" s="0" t="n">
+        <v>1801.45156121254</v>
+      </c>
+      <c r="G360" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H360" s="0" t="n">
+        <v>16.5087856952178</v>
+      </c>
+      <c r="I360" s="0" t="n">
+        <v>6.57355425619505</v>
+      </c>
+      <c r="J360" s="0" t="n">
+        <v>9.93523143902271</v>
+      </c>
+      <c r="K360" s="0" t="n">
+        <v>1.51139414870723</v>
+      </c>
+      <c r="L360" s="0" t="n">
+        <v>6.57355425619505</v>
+      </c>
+      <c r="M360" s="0" t="n">
+        <v>60.1814792586516</v>
+      </c>
+      <c r="P360" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q360" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="R360" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S360" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T360" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U360" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V360" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W360" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X360" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B361" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D361" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E361" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F361" s="0" t="n">
+        <v>1801.8295238018</v>
+      </c>
+      <c r="G361" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H361" s="0" t="n">
+        <v>16.6075200742542</v>
+      </c>
+      <c r="I361" s="0" t="n">
+        <v>6.98476347258359</v>
+      </c>
+      <c r="J361" s="0" t="n">
+        <v>9.62275660167057</v>
+      </c>
+      <c r="K361" s="0" t="n">
+        <v>1.37767823340641</v>
+      </c>
+      <c r="L361" s="0" t="n">
+        <v>6.98476347258359</v>
+      </c>
+      <c r="M361" s="0" t="n">
+        <v>57.9421645052729</v>
+      </c>
+      <c r="P361" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="Q361" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="R361" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S361" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T361" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U361" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="V361" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W361" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X361" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B362" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C362" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D362" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E362" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F362" s="0" t="n">
+        <v>1806.30399632454</v>
+      </c>
+      <c r="G362" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H362" s="0" t="n">
+        <v>10.7399313334654</v>
+      </c>
+      <c r="I362" s="0" t="n">
+        <v>4.83215301599565</v>
+      </c>
+      <c r="J362" s="0" t="n">
+        <v>5.90777831746977</v>
+      </c>
+      <c r="K362" s="0" t="n">
+        <v>1.2225975249363</v>
+      </c>
+      <c r="L362" s="0" t="n">
+        <v>4.83215301599565</v>
+      </c>
+      <c r="M362" s="0" t="n">
+        <v>55.0075985966618</v>
+      </c>
+      <c r="P362" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="Q362" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="R362" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S362" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T362" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U362" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V362" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W362" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X362" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D363" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E363" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F363" s="0" t="n">
+        <v>1801.74667429924</v>
+      </c>
+      <c r="G363" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H363" s="0" t="n">
+        <v>10.7399313334654</v>
+      </c>
+      <c r="I363" s="0" t="n">
+        <v>0.966786419776272</v>
+      </c>
+      <c r="J363" s="0" t="n">
+        <v>9.77314491368916</v>
+      </c>
+      <c r="K363" s="0" t="n">
+        <v>10.1088975949319</v>
+      </c>
+      <c r="L363" s="0" t="n">
+        <v>0.966786419776272</v>
+      </c>
+      <c r="M363" s="0" t="n">
+        <v>90.9982066946389</v>
+      </c>
+      <c r="P363" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="Q363" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="R363" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S363" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T363" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U363" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V363" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W363" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X363" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B364" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C364" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D364" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E364" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F364" s="0" t="n">
+        <v>1803.12563681603</v>
+      </c>
+      <c r="G364" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H364" s="0" t="n">
+        <v>12.94400052467</v>
+      </c>
+      <c r="I364" s="0" t="n">
+        <v>2.04335219960921</v>
+      </c>
+      <c r="J364" s="0" t="n">
+        <v>10.9006483250608</v>
+      </c>
+      <c r="K364" s="0" t="n">
+        <v>5.33468891322091</v>
+      </c>
+      <c r="L364" s="0" t="n">
+        <v>2.04335219960921</v>
+      </c>
+      <c r="M364" s="0" t="n">
+        <v>84.213905154633</v>
+      </c>
+      <c r="P364" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="Q364" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="R364" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S364" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T364" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U364" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V364" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W364" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X364" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B365" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C365" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D365" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E365" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F365" s="0" t="n">
+        <v>1803.65865397453</v>
+      </c>
+      <c r="G365" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H365" s="0" t="n">
+        <v>11.5109264272496</v>
+      </c>
+      <c r="I365" s="0" t="n">
+        <v>2.95101137175144</v>
+      </c>
+      <c r="J365" s="0" t="n">
+        <v>8.55991505549817</v>
+      </c>
+      <c r="K365" s="0" t="n">
+        <v>2.90067166037988</v>
+      </c>
+      <c r="L365" s="0" t="n">
+        <v>2.95101137175144</v>
+      </c>
+      <c r="M365" s="0" t="n">
+        <v>74.3633895116768</v>
+      </c>
+      <c r="P365" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="Q365" s="0" t="s">
+        <v>1152</v>
+      </c>
+      <c r="R365" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S365" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T365" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U365" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V365" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W365" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X365" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="0" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B366" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C366" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D366" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E366" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F366" s="0" t="n">
+        <v>1809.51467871666</v>
+      </c>
+      <c r="G366" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H366" s="0" t="n">
+        <v>5.56048112771352</v>
+      </c>
+      <c r="I366" s="0" t="n">
+        <v>1.56200545772862</v>
+      </c>
+      <c r="J366" s="0" t="n">
+        <v>3.9984756699849</v>
+      </c>
+      <c r="K366" s="0" t="n">
+        <v>2.55983463450842</v>
+      </c>
+      <c r="L366" s="0" t="n">
+        <v>1.56200545772862</v>
+      </c>
+      <c r="M366" s="0" t="n">
+        <v>71.9088074961075</v>
+      </c>
+      <c r="P366" s="0" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Q366" s="0" t="s">
+        <v>1156</v>
+      </c>
+      <c r="R366" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S366" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T366" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U366" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V366" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W366" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X366" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="0" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B367" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C367" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D367" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E367" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F367" s="0" t="n">
+        <v>1801.53783631325</v>
+      </c>
+      <c r="G367" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H367" s="0" t="n">
+        <v>7.26226100141758</v>
+      </c>
+      <c r="I367" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J367" s="0" t="n">
+        <v>7.26226100141758</v>
+      </c>
+      <c r="L367" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M367" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P367" s="0" t="s">
+        <v>1158</v>
+      </c>
+      <c r="Q367" s="0" t="s">
+        <v>1159</v>
+      </c>
+      <c r="R367" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S367" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T367" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U367" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V367" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W367" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X367" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="0" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B368" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C368" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D368" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E368" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F368" s="0" t="n">
+        <v>1802.71497106552</v>
+      </c>
+      <c r="G368" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H368" s="0" t="n">
+        <v>6.42046348337244</v>
+      </c>
+      <c r="I368" s="0" t="n">
+        <v>0.132133569400814</v>
+      </c>
+      <c r="J368" s="0" t="n">
+        <v>6.28832991397163</v>
+      </c>
+      <c r="K368" s="0" t="n">
+        <v>47.5907064532299</v>
+      </c>
+      <c r="L368" s="0" t="n">
+        <v>0.132133569400814</v>
+      </c>
+      <c r="M368" s="0" t="n">
+        <v>97.9419932884439</v>
+      </c>
+      <c r="P368" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Q368" s="0" t="s">
+        <v>1162</v>
+      </c>
+      <c r="R368" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S368" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T368" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U368" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V368" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W368" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X368" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="0" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B369" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C369" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D369" s="0" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E369" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F369" s="0" t="n">
+        <v>1803.85296845436</v>
+      </c>
+      <c r="G369" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H369" s="0" t="n">
+        <v>6.78448856833494</v>
+      </c>
+      <c r="I369" s="0" t="n">
+        <v>0.880069807711448</v>
+      </c>
+      <c r="J369" s="0" t="n">
+        <v>5.90441876062349</v>
+      </c>
+      <c r="K369" s="0" t="n">
+        <v>6.70903456622091</v>
+      </c>
+      <c r="L369" s="0" t="n">
+        <v>0.880069807711448</v>
+      </c>
+      <c r="M369" s="0" t="n">
+        <v>87.0282070807964</v>
+      </c>
+      <c r="P369" s="0" t="s">
+        <v>1164</v>
+      </c>
+      <c r="Q369" s="0" t="s">
+        <v>1165</v>
+      </c>
+      <c r="R369" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S369" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T369" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U369" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V369" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="W369" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X369" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B370" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C370" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D370" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E370" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F370" s="0" t="n">
+        <v>1808.05567622185</v>
+      </c>
+      <c r="G370" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H370" s="0" t="n">
+        <v>6.20896405349747</v>
+      </c>
+      <c r="I370" s="0" t="n">
+        <v>2.7194455651078</v>
+      </c>
+      <c r="J370" s="0" t="n">
+        <v>3.48951848838967</v>
+      </c>
+      <c r="K370" s="0" t="n">
+        <v>1.28317276622941</v>
+      </c>
+      <c r="L370" s="0" t="n">
+        <v>2.7194455651078</v>
+      </c>
+      <c r="M370" s="0" t="n">
+        <v>56.2012995778909</v>
+      </c>
+      <c r="P370" s="0" t="s">
+        <v>1168</v>
+      </c>
+      <c r="Q370" s="0" t="s">
+        <v>1169</v>
+      </c>
+      <c r="R370" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S370" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T370" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U370" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V370" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W370" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X370" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="0" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B371" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C371" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D371" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E371" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F371" s="0" t="n">
+        <v>1801.44995164871</v>
+      </c>
+      <c r="G371" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H371" s="0" t="n">
+        <v>9.24529359304578</v>
+      </c>
+      <c r="I371" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J371" s="0" t="n">
+        <v>9.24529359304578</v>
+      </c>
+      <c r="L371" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M371" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P371" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="Q371" s="0" t="s">
+        <v>1172</v>
+      </c>
+      <c r="R371" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S371" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T371" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U371" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V371" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W371" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X371" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B372" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C372" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D372" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E372" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F372" s="0" t="n">
+        <v>1802.73609447479</v>
+      </c>
+      <c r="G372" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H372" s="0" t="n">
+        <v>6.79941100341492</v>
+      </c>
+      <c r="I372" s="0" t="n">
+        <v>0.601580111306448</v>
+      </c>
+      <c r="J372" s="0" t="n">
+        <v>6.19783089210847</v>
+      </c>
+      <c r="K372" s="0" t="n">
+        <v>10.30258609888</v>
+      </c>
+      <c r="L372" s="0" t="n">
+        <v>0.601580111306448</v>
+      </c>
+      <c r="M372" s="0" t="n">
+        <v>91.1524673092374</v>
+      </c>
+      <c r="P372" s="0" t="s">
+        <v>1174</v>
+      </c>
+      <c r="Q372" s="0" t="s">
+        <v>1175</v>
+      </c>
+      <c r="R372" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S372" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T372" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U372" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V372" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W372" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X372" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="0" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B373" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C373" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D373" s="0" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E373" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F373" s="0" t="n">
+        <v>1803.51049137116</v>
+      </c>
+      <c r="G373" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H373" s="0" t="n">
+        <v>6.236860596489</v>
+      </c>
+      <c r="I373" s="0" t="n">
+        <v>1.11022222174015</v>
+      </c>
+      <c r="J373" s="0" t="n">
+        <v>5.12663837474884</v>
+      </c>
+      <c r="K373" s="0" t="n">
+        <v>4.61766867421677</v>
+      </c>
+      <c r="L373" s="0" t="n">
+        <v>1.11022222174015</v>
+      </c>
+      <c r="M373" s="0" t="n">
+        <v>82.1990213735875</v>
+      </c>
+      <c r="P373" s="0" t="s">
+        <v>1177</v>
+      </c>
+      <c r="Q373" s="0" t="s">
+        <v>1178</v>
+      </c>
+      <c r="R373" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S373" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T373" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U373" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V373" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W373" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X373" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B374" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C374" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D374" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E374" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F374" s="0" t="n">
+        <v>1809.49152207375</v>
+      </c>
+      <c r="G374" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H374" s="0" t="n">
+        <v>12.2176296696797</v>
+      </c>
+      <c r="I374" s="0" t="n">
+        <v>3.63407119298016</v>
+      </c>
+      <c r="J374" s="0" t="n">
+        <v>8.58355847669955</v>
+      </c>
+      <c r="K374" s="0" t="n">
+        <v>2.36196761727733</v>
+      </c>
+      <c r="L374" s="0" t="n">
+        <v>3.63407119298016</v>
+      </c>
+      <c r="M374" s="0" t="n">
+        <v>70.2555136206266</v>
+      </c>
+      <c r="P374" s="0" t="s">
+        <v>1181</v>
+      </c>
+      <c r="Q374" s="0" t="s">
+        <v>1182</v>
+      </c>
+      <c r="R374" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S374" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T374" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U374" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V374" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W374" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X374" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="0" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B375" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C375" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D375" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E375" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F375" s="0" t="n">
+        <v>1801.4968290329</v>
+      </c>
+      <c r="G375" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H375" s="0" t="n">
+        <v>14.6713882947304</v>
+      </c>
+      <c r="I375" s="0" t="n">
+        <v>0.608869726928325</v>
+      </c>
+      <c r="J375" s="0" t="n">
+        <v>14.0625185678021</v>
+      </c>
+      <c r="K375" s="0" t="n">
+        <v>23.0961040529077</v>
+      </c>
+      <c r="L375" s="0" t="n">
+        <v>0.608869726928325</v>
+      </c>
+      <c r="M375" s="0" t="n">
+        <v>95.8499515199457</v>
+      </c>
+      <c r="P375" s="0" t="s">
+        <v>1184</v>
+      </c>
+      <c r="Q375" s="0" t="s">
+        <v>1185</v>
+      </c>
+      <c r="R375" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S375" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T375" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U375" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V375" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W375" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X375" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="0" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B376" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C376" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D376" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E376" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F376" s="0" t="n">
+        <v>1803.34915041924</v>
+      </c>
+      <c r="G376" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H376" s="0" t="n">
+        <v>12.4281732178757</v>
+      </c>
+      <c r="I376" s="0" t="n">
+        <v>2.49926043663069</v>
+      </c>
+      <c r="J376" s="0" t="n">
+        <v>9.92891278124498</v>
+      </c>
+      <c r="K376" s="0" t="n">
+        <v>3.97274034979338</v>
+      </c>
+      <c r="L376" s="0" t="n">
+        <v>2.49926043663069</v>
+      </c>
+      <c r="M376" s="0" t="n">
+        <v>79.8903636695701</v>
+      </c>
+      <c r="P376" s="0" t="s">
+        <v>1187</v>
+      </c>
+      <c r="Q376" s="0" t="s">
+        <v>1188</v>
+      </c>
+      <c r="R376" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S376" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T376" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U376" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V376" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W376" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X376" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="0" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B377" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C377" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D377" s="0" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E377" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F377" s="0" t="n">
+        <v>1803.8495490551</v>
+      </c>
+      <c r="G377" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H377" s="0" t="n">
+        <v>13.3370885121027</v>
+      </c>
+      <c r="I377" s="0" t="n">
+        <v>3.04978706389849</v>
+      </c>
+      <c r="J377" s="0" t="n">
+        <v>10.2873014482042</v>
+      </c>
+      <c r="K377" s="0" t="n">
+        <v>3.37312121556911</v>
+      </c>
+      <c r="L377" s="0" t="n">
+        <v>3.04978706389849</v>
+      </c>
+      <c r="M377" s="0" t="n">
+        <v>77.1330372357433</v>
+      </c>
+      <c r="P377" s="0" t="s">
+        <v>1190</v>
+      </c>
+      <c r="Q377" s="0" t="s">
+        <v>1191</v>
+      </c>
+      <c r="R377" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S377" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T377" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U377" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="V377" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W377" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X377" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="0" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B378" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C378" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D378" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E378" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F378" s="0" t="n">
+        <v>1809.2066822052</v>
+      </c>
+      <c r="G378" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H378" s="0" t="n">
+        <v>7.13287368323651</v>
+      </c>
+      <c r="I378" s="0" t="n">
+        <v>2.77190543064587</v>
+      </c>
+      <c r="J378" s="0" t="n">
+        <v>4.36096825259065</v>
+      </c>
+      <c r="K378" s="0" t="n">
+        <v>1.57327454406499</v>
+      </c>
+      <c r="L378" s="0" t="n">
+        <v>2.77190543064587</v>
+      </c>
+      <c r="M378" s="0" t="n">
+        <v>61.1390085715337</v>
+      </c>
+      <c r="P378" s="0" t="s">
+        <v>1194</v>
+      </c>
+      <c r="Q378" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="R378" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S378" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T378" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U378" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V378" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W378" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X378" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B379" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C379" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D379" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E379" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F379" s="0" t="n">
+        <v>1801.53421902657</v>
+      </c>
+      <c r="G379" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H379" s="0" t="n">
+        <v>11.6634757583868</v>
+      </c>
+      <c r="I379" s="0" t="n">
+        <v>0.005551488750036</v>
+      </c>
+      <c r="J379" s="0" t="n">
+        <v>11.6579242696367</v>
+      </c>
+      <c r="K379" s="0" t="n">
+        <v>2099.96359437117</v>
+      </c>
+      <c r="L379" s="0" t="n">
+        <v>0.00555148875003631</v>
+      </c>
+      <c r="M379" s="0" t="n">
+        <v>99.952402792572</v>
+      </c>
+      <c r="P379" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="Q379" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="R379" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S379" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T379" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U379" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V379" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W379" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X379" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B380" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C380" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D380" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E380" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F380" s="0" t="n">
+        <v>1802.62905550003</v>
+      </c>
+      <c r="G380" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H380" s="0" t="n">
+        <v>6.98839741925852</v>
+      </c>
+      <c r="I380" s="0" t="n">
+        <v>1.17770931096333</v>
+      </c>
+      <c r="J380" s="0" t="n">
+        <v>5.81068810829519</v>
+      </c>
+      <c r="K380" s="0" t="n">
+        <v>4.93388992869746</v>
+      </c>
+      <c r="L380" s="0" t="n">
+        <v>1.17770931096333</v>
+      </c>
+      <c r="M380" s="0" t="n">
+        <v>83.147648304634</v>
+      </c>
+      <c r="P380" s="0" t="s">
+        <v>1200</v>
+      </c>
+      <c r="Q380" s="0" t="s">
+        <v>1201</v>
+      </c>
+      <c r="R380" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S380" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T380" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U380" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V380" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W380" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X380" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="0" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B381" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C381" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D381" s="0" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E381" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F381" s="0" t="n">
+        <v>1803.68817520142</v>
+      </c>
+      <c r="G381" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H381" s="0" t="n">
+        <v>7.85776200142866</v>
+      </c>
+      <c r="I381" s="0" t="n">
+        <v>0.688332819052256</v>
+      </c>
+      <c r="J381" s="0" t="n">
+        <v>7.16942918237641</v>
+      </c>
+      <c r="K381" s="0" t="n">
+        <v>10.4156433979826</v>
+      </c>
+      <c r="L381" s="0" t="n">
+        <v>0.688332819052256</v>
+      </c>
+      <c r="M381" s="0" t="n">
+        <v>91.2400907672298</v>
+      </c>
+      <c r="P381" s="0" t="s">
+        <v>1203</v>
+      </c>
+      <c r="Q381" s="0" t="s">
+        <v>1204</v>
+      </c>
+      <c r="R381" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S381" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T381" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U381" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V381" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="W381" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X381" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="0" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B382" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C382" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D382" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E382" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F382" s="0" t="n">
+        <v>1809.03082561493</v>
+      </c>
+      <c r="G382" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H382" s="0" t="n">
+        <v>11.3644425954758</v>
+      </c>
+      <c r="I382" s="0" t="n">
+        <v>3.69060326831486</v>
+      </c>
+      <c r="J382" s="0" t="n">
+        <v>7.67383932716091</v>
+      </c>
+      <c r="K382" s="0" t="n">
+        <v>2.07929131614973</v>
+      </c>
+      <c r="L382" s="0" t="n">
+        <v>3.69060326831486</v>
+      </c>
+      <c r="M382" s="0" t="n">
+        <v>67.5249952885142</v>
+      </c>
+      <c r="P382" s="0" t="s">
+        <v>1207</v>
+      </c>
+      <c r="Q382" s="0" t="s">
+        <v>1208</v>
+      </c>
+      <c r="R382" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S382" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T382" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U382" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V382" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W382" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X382" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B383" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C383" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D383" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E383" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F383" s="0" t="n">
+        <v>1801.65395522118</v>
+      </c>
+      <c r="G383" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H383" s="0" t="n">
+        <v>13.7925087599855</v>
+      </c>
+      <c r="I383" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J383" s="0" t="n">
+        <v>13.7925087599855</v>
+      </c>
+      <c r="L383" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M383" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P383" s="0" t="s">
+        <v>1210</v>
+      </c>
+      <c r="Q383" s="0" t="s">
+        <v>1211</v>
+      </c>
+      <c r="R383" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S383" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T383" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U383" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V383" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W383" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X383" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="0" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B384" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C384" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D384" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E384" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F384" s="0" t="n">
+        <v>1802.6246509552</v>
+      </c>
+      <c r="G384" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H384" s="0" t="n">
+        <v>12.4388303782786</v>
+      </c>
+      <c r="I384" s="0" t="n">
+        <v>0.068846240790615</v>
+      </c>
+      <c r="J384" s="0" t="n">
+        <v>12.3699841374879</v>
+      </c>
+      <c r="K384" s="0" t="n">
+        <v>179.675520339728</v>
+      </c>
+      <c r="L384" s="0" t="n">
+        <v>0.0688462407906145</v>
+      </c>
+      <c r="M384" s="0" t="n">
+        <v>99.4465215884699</v>
+      </c>
+      <c r="P384" s="0" t="s">
+        <v>1213</v>
+      </c>
+      <c r="Q384" s="0" t="s">
+        <v>1214</v>
+      </c>
+      <c r="R384" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S384" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T384" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U384" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V384" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W384" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X384" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B385" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C385" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D385" s="0" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E385" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F385" s="0" t="n">
+        <v>1804.20022273064</v>
+      </c>
+      <c r="G385" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H385" s="0" t="n">
+        <v>12.2537166062703</v>
+      </c>
+      <c r="I385" s="0" t="n">
+        <v>0.095724429648119</v>
+      </c>
+      <c r="J385" s="0" t="n">
+        <v>12.1579921766222</v>
+      </c>
+      <c r="K385" s="0" t="n">
+        <v>127.010338127004</v>
+      </c>
+      <c r="L385" s="0" t="n">
+        <v>0.0957244296481193</v>
+      </c>
+      <c r="M385" s="0" t="n">
+        <v>99.2188130938238</v>
+      </c>
+      <c r="P385" s="0" t="s">
+        <v>1216</v>
+      </c>
+      <c r="Q385" s="0" t="s">
+        <v>1217</v>
+      </c>
+      <c r="R385" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="S385" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T385" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="U385" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="V385" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="W385" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X385" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>